<commit_message>
Make some samples unused
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/uppsala_universitet/merce_temp_change/metadata.xlsx
+++ b/metadata/excel/projects/uppsala_universitet/merce_temp_change/metadata.xlsx
@@ -6093,10 +6093,10 @@
   </sheetPr>
   <dimension ref="A1:BZ211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="N185" sqref="N185"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>